<commit_message>
Added input file changes for to_report function
Added input file changes for to_report function. Added tabs: case_text_elements and generic_text_elements.
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -1,37 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lheringa001\Desktop\RBS_opensource\trbs_dsm\model\data\DSM\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isingh059\Documents\GitHub\trbs_main\src\vlinder\data\DSM\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E91D93-C97C-46C5-A426-D7D1DDD1917D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FDD34B-690F-47C6-BFEA-3352821E7C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22930" yWindow="-13960" windowWidth="30940" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
-    <sheet name="key_outputs" sheetId="2" r:id="rId2"/>
-    <sheet name="decision_makers_options" sheetId="3" r:id="rId3"/>
-    <sheet name="scenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="fixed_inputs" sheetId="5" r:id="rId5"/>
-    <sheet name="dependencies" sheetId="7" r:id="rId6"/>
-    <sheet name="theme_weights" sheetId="8" r:id="rId7"/>
-    <sheet name="key_output_weights" sheetId="9" r:id="rId8"/>
-    <sheet name="scenario_weights" sheetId="10" r:id="rId9"/>
+    <sheet name="case_text_elements" sheetId="11" r:id="rId2"/>
+    <sheet name="key_outputs" sheetId="2" r:id="rId3"/>
+    <sheet name="decision_makers_options" sheetId="3" r:id="rId4"/>
+    <sheet name="scenarios" sheetId="4" r:id="rId5"/>
+    <sheet name="fixed_inputs" sheetId="5" r:id="rId6"/>
+    <sheet name="dependencies" sheetId="7" r:id="rId7"/>
+    <sheet name="theme_weights" sheetId="8" r:id="rId8"/>
+    <sheet name="key_output_weights" sheetId="9" r:id="rId9"/>
+    <sheet name="scenario_weights" sheetId="10" r:id="rId10"/>
+    <sheet name="generic_text_elements" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">dependencies!$A$1:$H$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">dependencies!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="156">
   <si>
     <t>configuration</t>
   </si>
@@ -409,6 +411,96 @@
   </si>
   <si>
     <t>Total demand RS and RE</t>
+  </si>
+  <si>
+    <t>case_text_element</t>
+  </si>
+  <si>
+    <t>title_front_page</t>
+  </si>
+  <si>
+    <t>strategic_challenge</t>
+  </si>
+  <si>
+    <t>Report of the DSM case</t>
+  </si>
+  <si>
+    <t>How to source energy?</t>
+  </si>
+  <si>
+    <t>generic_text_element</t>
+  </si>
+  <si>
+    <t>title_strategic_challenge</t>
+  </si>
+  <si>
+    <t>Strategic Challenge</t>
+  </si>
+  <si>
+    <t>title_key_outputs</t>
+  </si>
+  <si>
+    <t>Key outputs</t>
+  </si>
+  <si>
+    <t>title_dmo</t>
+  </si>
+  <si>
+    <t>Decision makers options (DMOs)</t>
+  </si>
+  <si>
+    <t>title_scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>title_fixed_inputs</t>
+  </si>
+  <si>
+    <t>Fixed inputs</t>
+  </si>
+  <si>
+    <t>title_dependency_graph</t>
+  </si>
+  <si>
+    <t>Dependency graph</t>
+  </si>
+  <si>
+    <t>title_weighted_graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resulting appreciations of different DMOs for scenario: </t>
+  </si>
+  <si>
+    <t>intro_key_outputs</t>
+  </si>
+  <si>
+    <t>The outputs upon which the decision makers will base their decision. Key outputs are often referred to as KPIs. Key outputs are grouped into themes.</t>
+  </si>
+  <si>
+    <t>intro_dmo</t>
+  </si>
+  <si>
+    <t>Decision makers options are formulated by assigning a single value to all internal variable inputs. These inputs can be formulated and determined by the decision makers.</t>
+  </si>
+  <si>
+    <t>intro_scenarios</t>
+  </si>
+  <si>
+    <t>Each external variable input can be thought of as a single aspect of external uncertainty affecting the outcome of the decision in scope. A scenario is defined by assigning a single value to all external variable inputs.</t>
+  </si>
+  <si>
+    <t>intro_fixed_inputs</t>
+  </si>
+  <si>
+    <t>The inputs which only takes one value for all scenarios.</t>
+  </si>
+  <si>
+    <t>intro_dependency_graph</t>
+  </si>
+  <si>
+    <t>intro_weighted_graph</t>
   </si>
 </sst>
 </file>
@@ -419,7 +511,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +570,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -493,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -542,12 +654,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -602,6 +727,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -911,12 +1046,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -937,7 +1072,227 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D82725-75FE-4DA5-A921-89C7E0B81CFF}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="25"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0B2266-EF72-405E-80DD-C68DEEE32A88}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -945,20 +1300,20 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -987,7 +1342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
@@ -1014,7 +1369,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
@@ -1041,7 +1396,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1423,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -1095,7 +1450,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -1122,7 +1477,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>36</v>
       </c>
@@ -1149,7 +1504,7 @@
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
@@ -1176,7 +1531,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
@@ -1203,7 +1558,7 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
@@ -1236,19 +1591,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1259,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1270,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1281,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1303,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>111</v>
       </c>
@@ -1314,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
@@ -1325,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
@@ -1336,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1347,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -1358,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1369,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1380,7 +1735,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>111</v>
       </c>
@@ -1391,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>110</v>
       </c>
@@ -1402,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>112</v>
       </c>
@@ -1413,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1424,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1435,7 +1790,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -1446,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>111</v>
       </c>
@@ -1468,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -1479,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>112</v>
       </c>
@@ -1490,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1501,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -1512,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1878,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1889,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
@@ -1545,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>110</v>
       </c>
@@ -1556,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -1567,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1578,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
@@ -1589,7 +1944,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1600,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +1966,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>111</v>
       </c>
@@ -1622,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>110</v>
       </c>
@@ -1633,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
@@ -1644,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1656,7 +2011,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1668,7 +2023,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1680,7 +2035,7 @@
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1692,7 +2047,7 @@
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
@@ -1704,7 +2059,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -1716,7 +2071,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>112</v>
       </c>
@@ -1736,7 +2091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -1744,14 +2099,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1762,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +2128,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -1784,7 +2139,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +2150,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1806,7 +2161,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
@@ -1817,7 +2172,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>53</v>
       </c>
@@ -1828,7 +2183,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -1839,7 +2194,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -1850,7 +2205,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -1861,7 +2216,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -1872,7 +2227,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
@@ -1883,7 +2238,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -1894,7 +2249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -1905,7 +2260,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -1916,7 +2271,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -1927,7 +2282,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
@@ -1938,7 +2293,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -1949,7 +2304,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +2315,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
@@ -1971,7 +2326,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
@@ -1982,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
@@ -1998,7 +2353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -2006,12 +2361,12 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2027,7 +2382,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2035,7 +2390,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -2043,7 +2398,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -2051,7 +2406,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2059,7 +2414,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -2067,7 +2422,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2075,7 +2430,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -2083,7 +2438,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -2091,7 +2446,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2099,7 +2454,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -2107,7 +2462,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -2115,7 +2470,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -2123,7 +2478,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -2131,172 +2486,172 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="7"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="7"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="7"/>
     </row>
   </sheetData>
@@ -2304,27 +2659,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -2364,7 +2719,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -2378,7 +2733,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>73</v>
       </c>
@@ -2406,7 +2761,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
@@ -2420,7 +2775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>124</v>
       </c>
@@ -2434,7 +2789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>124</v>
       </c>
@@ -2448,7 +2803,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>74</v>
       </c>
@@ -2462,7 +2817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2476,7 +2831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>31</v>
       </c>
@@ -2490,7 +2845,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>75</v>
       </c>
@@ -2504,7 +2859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>76</v>
       </c>
@@ -2518,7 +2873,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>77</v>
       </c>
@@ -2532,7 +2887,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>78</v>
       </c>
@@ -2546,7 +2901,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
@@ -2560,7 +2915,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>80</v>
       </c>
@@ -2574,7 +2929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>81</v>
       </c>
@@ -2588,7 +2943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>82</v>
       </c>
@@ -2602,7 +2957,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
@@ -2616,7 +2971,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>84</v>
       </c>
@@ -2630,7 +2985,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>85</v>
       </c>
@@ -2644,7 +2999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>86</v>
       </c>
@@ -2658,7 +3013,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>87</v>
       </c>
@@ -2672,7 +3027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>88</v>
       </c>
@@ -2686,7 +3041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +3055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>89</v>
       </c>
@@ -2714,7 +3069,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>90</v>
       </c>
@@ -2728,7 +3083,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>91</v>
       </c>
@@ -2742,7 +3097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>91</v>
       </c>
@@ -2756,7 +3111,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>125</v>
       </c>
@@ -2770,7 +3125,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>125</v>
       </c>
@@ -2784,7 +3139,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
@@ -2798,7 +3153,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>93</v>
       </c>
@@ -2812,7 +3167,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>94</v>
       </c>
@@ -2826,7 +3181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>104</v>
       </c>
@@ -2840,7 +3195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>104</v>
       </c>
@@ -2854,7 +3209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>105</v>
       </c>
@@ -2868,7 +3223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>106</v>
       </c>
@@ -2882,7 +3237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>106</v>
       </c>
@@ -2896,7 +3251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>107</v>
       </c>
@@ -2910,7 +3265,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>95</v>
       </c>
@@ -2924,7 +3279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>95</v>
       </c>
@@ -2938,7 +3293,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
@@ -2952,7 +3307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
@@ -2966,7 +3321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>97</v>
       </c>
@@ -2980,7 +3335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>32</v>
       </c>
@@ -2994,7 +3349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>32</v>
       </c>
@@ -3008,7 +3363,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>32</v>
       </c>
@@ -3022,7 +3377,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>33</v>
       </c>
@@ -3036,7 +3391,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>33</v>
       </c>
@@ -3050,7 +3405,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>98</v>
       </c>
@@ -3064,7 +3419,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>34</v>
       </c>
@@ -3078,7 +3433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>34</v>
       </c>
@@ -3092,7 +3447,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>39</v>
       </c>
@@ -3106,7 +3461,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>100</v>
       </c>
@@ -3120,7 +3475,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>36</v>
       </c>
@@ -3134,7 +3489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
         <v>108</v>
       </c>
@@ -3150,7 +3505,7 @@
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
         <v>122</v>
       </c>
@@ -3166,7 +3521,7 @@
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>123</v>
       </c>
@@ -3182,7 +3537,7 @@
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
         <v>101</v>
       </c>
@@ -3198,7 +3553,7 @@
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
         <v>101</v>
       </c>
@@ -3214,7 +3569,7 @@
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="s">
         <v>109</v>
       </c>
@@ -3230,7 +3585,7 @@
       <c r="E63" s="17"/>
       <c r="F63" s="17"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
         <v>109</v>
       </c>
@@ -3246,7 +3601,7 @@
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
         <v>37</v>
       </c>
@@ -3262,7 +3617,7 @@
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>99</v>
       </c>
@@ -3278,7 +3633,7 @@
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
         <v>102</v>
       </c>
@@ -3294,7 +3649,7 @@
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
         <v>102</v>
       </c>
@@ -3310,7 +3665,7 @@
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="s">
         <v>102</v>
       </c>
@@ -3326,15 +3681,15 @@
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -3348,7 +3703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3356,9 +3711,9 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3366,7 +3721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3374,7 +3729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3382,7 +3737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3395,7 +3750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3403,13 +3758,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3417,7 +3772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
@@ -3425,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
@@ -3433,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
@@ -3441,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -3449,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -3457,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>36</v>
       </c>
@@ -3465,7 +3820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
@@ -3473,7 +3828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
@@ -3481,61 +3836,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="15">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add text files for other cases and formats
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -1,37 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lheringa001\Desktop\RBS_opensource\trbs_dsm\model\data\DSM\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E91D93-C97C-46C5-A426-D7D1DDD1917D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDD0B1E-C7CC-4C40-A40F-48BBBD72638E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
-    <sheet name="key_outputs" sheetId="2" r:id="rId2"/>
-    <sheet name="decision_makers_options" sheetId="3" r:id="rId3"/>
-    <sheet name="scenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="fixed_inputs" sheetId="5" r:id="rId5"/>
-    <sheet name="dependencies" sheetId="7" r:id="rId6"/>
-    <sheet name="theme_weights" sheetId="8" r:id="rId7"/>
-    <sheet name="key_output_weights" sheetId="9" r:id="rId8"/>
-    <sheet name="scenario_weights" sheetId="10" r:id="rId9"/>
+    <sheet name="generic_text_elements" sheetId="11" r:id="rId2"/>
+    <sheet name="case_text_elements" sheetId="12" r:id="rId3"/>
+    <sheet name="key_outputs" sheetId="2" r:id="rId4"/>
+    <sheet name="decision_makers_options" sheetId="3" r:id="rId5"/>
+    <sheet name="scenarios" sheetId="4" r:id="rId6"/>
+    <sheet name="fixed_inputs" sheetId="5" r:id="rId7"/>
+    <sheet name="dependencies" sheetId="7" r:id="rId8"/>
+    <sheet name="theme_weights" sheetId="8" r:id="rId9"/>
+    <sheet name="key_output_weights" sheetId="9" r:id="rId10"/>
+    <sheet name="scenario_weights" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">dependencies!$A$1:$H$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">dependencies!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="152">
   <si>
     <t>configuration</t>
   </si>
@@ -409,6 +411,84 @@
   </si>
   <si>
     <t>Total demand RS and RE</t>
+  </si>
+  <si>
+    <t>generic_text_element</t>
+  </si>
+  <si>
+    <t>title_strategic_challenge</t>
+  </si>
+  <si>
+    <t>Strategic Challenge</t>
+  </si>
+  <si>
+    <t>title_key_outputs</t>
+  </si>
+  <si>
+    <t>Key outputs</t>
+  </si>
+  <si>
+    <t>title_dmo</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>title_scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>title_comparison</t>
+  </si>
+  <si>
+    <t>Comparisons of options</t>
+  </si>
+  <si>
+    <t>title_theme_weights</t>
+  </si>
+  <si>
+    <t>Key output and theme weights</t>
+  </si>
+  <si>
+    <t>title_scenario_weights</t>
+  </si>
+  <si>
+    <t>Scenario weights</t>
+  </si>
+  <si>
+    <t>text_strategic_challenge</t>
+  </si>
+  <si>
+    <t>Describing strategic challenge that requires a decision</t>
+  </si>
+  <si>
+    <t>text_key_outputs</t>
+  </si>
+  <si>
+    <t>Which indicators do you use to evaluate the impact of your decision(s)?</t>
+  </si>
+  <si>
+    <t>text_dmo</t>
+  </si>
+  <si>
+    <t>Which options do you have to influence your impact?</t>
+  </si>
+  <si>
+    <t>text_scenarios</t>
+  </si>
+  <si>
+    <t>Which uncertainty do you want to account for?</t>
+  </si>
+  <si>
+    <t>case_text_element</t>
+  </si>
+  <si>
+    <t>strategic_challenge</t>
+  </si>
+  <si>
+    <t>How to source energy?</t>
   </si>
 </sst>
 </file>
@@ -419,9 +499,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -431,6 +518,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -443,6 +531,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -460,17 +549,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -479,7 +571,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,6 +581,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,69 +641,71 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{AE53C5E1-75E6-4245-B0B1-466E5639B5C7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -911,12 +1011,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,12 +1024,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -938,6 +1187,161 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E1CC75-D97A-4B40-BEB4-D0908A445A81}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AD5AE-B0E9-A747-915F-4F9B572E98DB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -945,20 +1349,20 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -987,248 +1391,239 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>-41400000</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>30000000</v>
       </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>5734800</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>8389800</v>
       </c>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
         <v>0.1</v>
       </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
         <v>3988.3999999999942</v>
       </c>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>39884</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>39884</v>
       </c>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
         <v>1.73</v>
       </c>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
         <v>1.1244999999999998</v>
       </c>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
         <v>0.17300000000000001</v>
       </c>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
         <v>845540.79999999877</v>
       </c>
-      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1236,19 +1631,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1259,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1270,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1281,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1303,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>111</v>
       </c>
@@ -1314,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
@@ -1325,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
@@ -1336,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1347,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -1358,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1369,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1380,7 +1775,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>111</v>
       </c>
@@ -1391,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>110</v>
       </c>
@@ -1402,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>112</v>
       </c>
@@ -1413,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1424,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1435,7 +1830,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -1446,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>111</v>
       </c>
@@ -1468,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -1479,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>112</v>
       </c>
@@ -1490,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1501,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -1512,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1918,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1929,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
@@ -1545,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>110</v>
       </c>
@@ -1556,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -1567,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1578,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
@@ -1589,7 +1984,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1600,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +2006,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>111</v>
       </c>
@@ -1622,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>110</v>
       </c>
@@ -1633,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
@@ -1644,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1656,7 +2051,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1668,7 +2063,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1680,7 +2075,7 @@
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1692,7 +2087,7 @@
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
@@ -1704,7 +2099,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -1716,7 +2111,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>112</v>
       </c>
@@ -1736,7 +2131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -1744,14 +2139,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1762,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +2168,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -1784,7 +2179,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +2190,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1806,7 +2201,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
@@ -1817,7 +2212,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>53</v>
       </c>
@@ -1828,7 +2223,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -1839,7 +2234,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -1850,7 +2245,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -1861,7 +2256,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -1872,7 +2267,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
@@ -1883,7 +2278,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -1894,7 +2289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -1905,7 +2300,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -1916,7 +2311,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -1927,7 +2322,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
@@ -1938,7 +2333,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -1949,7 +2344,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +2355,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
@@ -1971,7 +2366,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
@@ -1982,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
@@ -1998,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -2006,12 +2401,12 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2027,7 +2422,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2035,7 +2430,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -2043,7 +2438,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -2051,7 +2446,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2059,7 +2454,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -2067,7 +2462,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2075,7 +2470,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -2083,7 +2478,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -2091,7 +2486,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2099,7 +2494,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -2107,7 +2502,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -2115,7 +2510,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -2123,7 +2518,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -2131,172 +2526,172 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
     </row>
   </sheetData>
@@ -2304,27 +2699,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -2364,7 +2759,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -2378,7 +2773,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>73</v>
       </c>
@@ -2406,49 +2801,49 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>74</v>
       </c>
@@ -2462,7 +2857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2476,21 +2871,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>75</v>
       </c>
@@ -2504,7 +2899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>76</v>
       </c>
@@ -2518,7 +2913,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>77</v>
       </c>
@@ -2532,7 +2927,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>78</v>
       </c>
@@ -2546,7 +2941,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
@@ -2560,7 +2955,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>80</v>
       </c>
@@ -2574,7 +2969,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>81</v>
       </c>
@@ -2588,7 +2983,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>82</v>
       </c>
@@ -2602,7 +2997,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
@@ -2616,7 +3011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>84</v>
       </c>
@@ -2630,7 +3025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>85</v>
       </c>
@@ -2644,7 +3039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>86</v>
       </c>
@@ -2658,7 +3053,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>87</v>
       </c>
@@ -2672,7 +3067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>88</v>
       </c>
@@ -2686,7 +3081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +3095,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>89</v>
       </c>
@@ -2714,7 +3109,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>90</v>
       </c>
@@ -2728,7 +3123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>91</v>
       </c>
@@ -2742,7 +3137,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>91</v>
       </c>
@@ -2756,7 +3151,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>125</v>
       </c>
@@ -2770,7 +3165,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>125</v>
       </c>
@@ -2784,7 +3179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
@@ -2798,21 +3193,21 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>125</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>94</v>
       </c>
@@ -2826,7 +3221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>104</v>
       </c>
@@ -2840,7 +3235,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>104</v>
       </c>
@@ -2854,7 +3249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>105</v>
       </c>
@@ -2868,7 +3263,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>106</v>
       </c>
@@ -2882,7 +3277,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>106</v>
       </c>
@@ -2896,7 +3291,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>107</v>
       </c>
@@ -2910,7 +3305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>95</v>
       </c>
@@ -2924,7 +3319,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>95</v>
       </c>
@@ -2938,7 +3333,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
@@ -2952,7 +3347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
@@ -2966,7 +3361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>97</v>
       </c>
@@ -2980,7 +3375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>32</v>
       </c>
@@ -2994,7 +3389,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>32</v>
       </c>
@@ -3008,7 +3403,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>32</v>
       </c>
@@ -3022,7 +3417,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>33</v>
       </c>
@@ -3036,7 +3431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>33</v>
       </c>
@@ -3050,7 +3445,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>98</v>
       </c>
@@ -3064,7 +3459,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>34</v>
       </c>
@@ -3078,7 +3473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>34</v>
       </c>
@@ -3092,21 +3487,21 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>100</v>
       </c>
@@ -3120,149 +3515,149 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+    </row>
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="15">
         <v>1</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="15">
         <v>1</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+    </row>
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+    </row>
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+    </row>
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+    </row>
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>99</v>
       </c>
@@ -3275,11 +3670,11 @@
       <c r="D66" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B67" s="11" t="s">
@@ -3291,56 +3686,56 @@
       <c r="D67" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="16">
-        <v>0</v>
-      </c>
-      <c r="C68" s="16" t="s">
+      <c r="B68" s="15">
+        <v>0</v>
+      </c>
+      <c r="C68" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3348,7 +3743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3356,9 +3751,9 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3366,7 +3761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3374,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3382,160 +3777,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add generic and case text elements to input xlsx for beerwiser (#37)
* add generic and case text elements to input xlsx for beerwiser

* add text files for other cases and formats

* add text files for other cases and formats

* Update pyproject.toml
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -1,37 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lheringa001\Desktop\RBS_opensource\trbs_dsm\model\data\DSM\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E91D93-C97C-46C5-A426-D7D1DDD1917D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDD0B1E-C7CC-4C40-A40F-48BBBD72638E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
-    <sheet name="key_outputs" sheetId="2" r:id="rId2"/>
-    <sheet name="decision_makers_options" sheetId="3" r:id="rId3"/>
-    <sheet name="scenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="fixed_inputs" sheetId="5" r:id="rId5"/>
-    <sheet name="dependencies" sheetId="7" r:id="rId6"/>
-    <sheet name="theme_weights" sheetId="8" r:id="rId7"/>
-    <sheet name="key_output_weights" sheetId="9" r:id="rId8"/>
-    <sheet name="scenario_weights" sheetId="10" r:id="rId9"/>
+    <sheet name="generic_text_elements" sheetId="11" r:id="rId2"/>
+    <sheet name="case_text_elements" sheetId="12" r:id="rId3"/>
+    <sheet name="key_outputs" sheetId="2" r:id="rId4"/>
+    <sheet name="decision_makers_options" sheetId="3" r:id="rId5"/>
+    <sheet name="scenarios" sheetId="4" r:id="rId6"/>
+    <sheet name="fixed_inputs" sheetId="5" r:id="rId7"/>
+    <sheet name="dependencies" sheetId="7" r:id="rId8"/>
+    <sheet name="theme_weights" sheetId="8" r:id="rId9"/>
+    <sheet name="key_output_weights" sheetId="9" r:id="rId10"/>
+    <sheet name="scenario_weights" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">dependencies!$A$1:$H$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">dependencies!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="152">
   <si>
     <t>configuration</t>
   </si>
@@ -409,6 +411,84 @@
   </si>
   <si>
     <t>Total demand RS and RE</t>
+  </si>
+  <si>
+    <t>generic_text_element</t>
+  </si>
+  <si>
+    <t>title_strategic_challenge</t>
+  </si>
+  <si>
+    <t>Strategic Challenge</t>
+  </si>
+  <si>
+    <t>title_key_outputs</t>
+  </si>
+  <si>
+    <t>Key outputs</t>
+  </si>
+  <si>
+    <t>title_dmo</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>title_scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>title_comparison</t>
+  </si>
+  <si>
+    <t>Comparisons of options</t>
+  </si>
+  <si>
+    <t>title_theme_weights</t>
+  </si>
+  <si>
+    <t>Key output and theme weights</t>
+  </si>
+  <si>
+    <t>title_scenario_weights</t>
+  </si>
+  <si>
+    <t>Scenario weights</t>
+  </si>
+  <si>
+    <t>text_strategic_challenge</t>
+  </si>
+  <si>
+    <t>Describing strategic challenge that requires a decision</t>
+  </si>
+  <si>
+    <t>text_key_outputs</t>
+  </si>
+  <si>
+    <t>Which indicators do you use to evaluate the impact of your decision(s)?</t>
+  </si>
+  <si>
+    <t>text_dmo</t>
+  </si>
+  <si>
+    <t>Which options do you have to influence your impact?</t>
+  </si>
+  <si>
+    <t>text_scenarios</t>
+  </si>
+  <si>
+    <t>Which uncertainty do you want to account for?</t>
+  </si>
+  <si>
+    <t>case_text_element</t>
+  </si>
+  <si>
+    <t>strategic_challenge</t>
+  </si>
+  <si>
+    <t>How to source energy?</t>
   </si>
 </sst>
 </file>
@@ -419,9 +499,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -431,6 +518,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -443,6 +531,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -460,17 +549,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -479,7 +571,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,6 +581,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,69 +641,71 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{AE53C5E1-75E6-4245-B0B1-466E5639B5C7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -911,12 +1011,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,12 +1024,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -938,6 +1187,161 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E1CC75-D97A-4B40-BEB4-D0908A445A81}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AD5AE-B0E9-A747-915F-4F9B572E98DB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -945,20 +1349,20 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -987,248 +1391,239 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>-41400000</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>30000000</v>
       </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>5734800</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>8389800</v>
       </c>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
         <v>0.1</v>
       </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
         <v>3988.3999999999942</v>
       </c>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>39884</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>39884</v>
       </c>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
         <v>1.73</v>
       </c>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
         <v>1.1244999999999998</v>
       </c>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
         <v>0.17300000000000001</v>
       </c>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
         <v>845540.79999999877</v>
       </c>
-      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1236,19 +1631,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1259,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1270,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1281,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1303,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>111</v>
       </c>
@@ -1314,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
@@ -1325,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
@@ -1336,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1347,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -1358,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1369,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1380,7 +1775,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>111</v>
       </c>
@@ -1391,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>110</v>
       </c>
@@ -1402,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>112</v>
       </c>
@@ -1413,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1424,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1435,7 +1830,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -1446,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>111</v>
       </c>
@@ -1468,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -1479,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>112</v>
       </c>
@@ -1490,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1501,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -1512,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1918,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1929,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
@@ -1545,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>110</v>
       </c>
@@ -1556,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -1567,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1578,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
@@ -1589,7 +1984,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1600,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +2006,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>111</v>
       </c>
@@ -1622,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>110</v>
       </c>
@@ -1633,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
@@ -1644,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1656,7 +2051,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1668,7 +2063,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1680,7 +2075,7 @@
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1692,7 +2087,7 @@
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
@@ -1704,7 +2099,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>110</v>
       </c>
@@ -1716,7 +2111,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>112</v>
       </c>
@@ -1736,7 +2131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -1744,14 +2139,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1762,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +2168,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -1784,7 +2179,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +2190,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1806,7 +2201,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
@@ -1817,7 +2212,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>53</v>
       </c>
@@ -1828,7 +2223,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -1839,7 +2234,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -1850,7 +2245,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -1861,7 +2256,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -1872,7 +2267,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
@@ -1883,7 +2278,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -1894,7 +2289,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -1905,7 +2300,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -1916,7 +2311,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
@@ -1927,7 +2322,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
@@ -1938,7 +2333,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -1949,7 +2344,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +2355,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
@@ -1971,7 +2366,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>53</v>
       </c>
@@ -1982,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>54</v>
       </c>
@@ -1998,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -2006,12 +2401,12 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2027,7 +2422,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2035,7 +2430,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -2043,7 +2438,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -2051,7 +2446,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2059,7 +2454,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -2067,7 +2462,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2075,7 +2470,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -2083,7 +2478,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -2091,7 +2486,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2099,7 +2494,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -2107,7 +2502,7 @@
         <v>1.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -2115,7 +2510,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -2123,7 +2518,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -2131,172 +2526,172 @@
         <v>40000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
     </row>
   </sheetData>
@@ -2304,27 +2699,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -2364,7 +2759,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -2378,7 +2773,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>73</v>
       </c>
@@ -2406,49 +2801,49 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>74</v>
       </c>
@@ -2462,7 +2857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>103</v>
       </c>
@@ -2476,21 +2871,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>75</v>
       </c>
@@ -2504,7 +2899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>76</v>
       </c>
@@ -2518,7 +2913,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>77</v>
       </c>
@@ -2532,7 +2927,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>78</v>
       </c>
@@ -2546,7 +2941,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
@@ -2560,7 +2955,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>80</v>
       </c>
@@ -2574,7 +2969,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>81</v>
       </c>
@@ -2588,7 +2983,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>82</v>
       </c>
@@ -2602,7 +2997,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
@@ -2616,7 +3011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>84</v>
       </c>
@@ -2630,7 +3025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>85</v>
       </c>
@@ -2644,7 +3039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>86</v>
       </c>
@@ -2658,7 +3053,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>87</v>
       </c>
@@ -2672,7 +3067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>88</v>
       </c>
@@ -2686,7 +3081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +3095,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>89</v>
       </c>
@@ -2714,7 +3109,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>90</v>
       </c>
@@ -2728,7 +3123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>91</v>
       </c>
@@ -2742,7 +3137,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>91</v>
       </c>
@@ -2756,7 +3151,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>125</v>
       </c>
@@ -2770,7 +3165,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>125</v>
       </c>
@@ -2784,7 +3179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>125</v>
       </c>
@@ -2798,21 +3193,21 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>125</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>94</v>
       </c>
@@ -2826,7 +3221,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>104</v>
       </c>
@@ -2840,7 +3235,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>104</v>
       </c>
@@ -2854,7 +3249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>105</v>
       </c>
@@ -2868,7 +3263,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>106</v>
       </c>
@@ -2882,7 +3277,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>106</v>
       </c>
@@ -2896,7 +3291,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>107</v>
       </c>
@@ -2910,7 +3305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>95</v>
       </c>
@@ -2924,7 +3319,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>95</v>
       </c>
@@ -2938,7 +3333,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
@@ -2952,7 +3347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
@@ -2966,7 +3361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>97</v>
       </c>
@@ -2980,7 +3375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>32</v>
       </c>
@@ -2994,7 +3389,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>32</v>
       </c>
@@ -3008,7 +3403,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>32</v>
       </c>
@@ -3022,7 +3417,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>33</v>
       </c>
@@ -3036,7 +3431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>33</v>
       </c>
@@ -3050,7 +3445,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>98</v>
       </c>
@@ -3064,7 +3459,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>34</v>
       </c>
@@ -3078,7 +3473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>34</v>
       </c>
@@ -3092,21 +3487,21 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>100</v>
       </c>
@@ -3120,149 +3515,149 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+    </row>
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="15">
         <v>1</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="16">
+      <c r="B60" s="15">
         <v>1</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+    </row>
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+    </row>
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+    </row>
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+    </row>
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>99</v>
       </c>
@@ -3275,11 +3670,11 @@
       <c r="D66" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B67" s="11" t="s">
@@ -3291,56 +3686,56 @@
       <c r="D67" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="16">
-        <v>0</v>
-      </c>
-      <c r="C68" s="16" t="s">
+      <c r="B68" s="15">
+        <v>0</v>
+      </c>
+      <c r="C68" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3348,7 +3743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3356,9 +3751,9 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3366,7 +3761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3374,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3382,160 +3777,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
alter generic and case specific texts
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDD0B1E-C7CC-4C40-A40F-48BBBD72638E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE116A6-F48F-6242-807A-86AD9CBFE2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="-20360" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="189">
   <si>
     <t>configuration</t>
   </si>
@@ -419,9 +419,6 @@
     <t>title_strategic_challenge</t>
   </si>
   <si>
-    <t>Strategic Challenge</t>
-  </si>
-  <si>
     <t>title_key_outputs</t>
   </si>
   <si>
@@ -440,55 +437,170 @@
     <t>Scenarios</t>
   </si>
   <si>
-    <t>title_comparison</t>
-  </si>
-  <si>
-    <t>Comparisons of options</t>
-  </si>
-  <si>
-    <t>title_theme_weights</t>
-  </si>
-  <si>
-    <t>Key output and theme weights</t>
-  </si>
-  <si>
-    <t>title_scenario_weights</t>
-  </si>
-  <si>
-    <t>Scenario weights</t>
-  </si>
-  <si>
     <t>text_strategic_challenge</t>
   </si>
   <si>
-    <t>Describing strategic challenge that requires a decision</t>
-  </si>
-  <si>
     <t>text_key_outputs</t>
   </si>
   <si>
-    <t>Which indicators do you use to evaluate the impact of your decision(s)?</t>
-  </si>
-  <si>
     <t>text_dmo</t>
   </si>
   <si>
-    <t>Which options do you have to influence your impact?</t>
-  </si>
-  <si>
     <t>text_scenarios</t>
   </si>
   <si>
-    <t>Which uncertainty do you want to account for?</t>
-  </si>
-  <si>
     <t>case_text_element</t>
   </si>
   <si>
     <t>strategic_challenge</t>
   </si>
   <si>
-    <t>How to source energy?</t>
+    <t>Strategic challenge</t>
+  </si>
+  <si>
+    <t>title_comparison_dmo</t>
+  </si>
+  <si>
+    <t>Strategic priorities</t>
+  </si>
+  <si>
+    <t>title_comparison_scenario</t>
+  </si>
+  <si>
+    <t>Risk appetite</t>
+  </si>
+  <si>
+    <t>title_fixed_inputs</t>
+  </si>
+  <si>
+    <t>Fixed inputs</t>
+  </si>
+  <si>
+    <t>title_dependency_graph</t>
+  </si>
+  <si>
+    <t>Dependency graph</t>
+  </si>
+  <si>
+    <t>title_weighted_graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resulting appreciations of different DMOs for scenario: </t>
+  </si>
+  <si>
+    <t>The strategic challenge that requires a decision</t>
+  </si>
+  <si>
+    <t>The indicators used to evaluate the impact of your decision</t>
+  </si>
+  <si>
+    <t>The options you have to influence your impact</t>
+  </si>
+  <si>
+    <t>The uncertainty you want to account for</t>
+  </si>
+  <si>
+    <t>text_comparison_dmo</t>
+  </si>
+  <si>
+    <t>Evaluate options by assessing strategic priorities</t>
+  </si>
+  <si>
+    <t>text_comparison_scenario</t>
+  </si>
+  <si>
+    <t>Evaluate options by assessing risk appetite</t>
+  </si>
+  <si>
+    <t>intro_key_outputs</t>
+  </si>
+  <si>
+    <t>The outputs upon which the decision makers will base their decision. Key outputs are often referred to as KPIs. Key outputs are grouped into themes.</t>
+  </si>
+  <si>
+    <t>intro_decision_makers_options</t>
+  </si>
+  <si>
+    <t>Decision makers options are formulated by assigning a single value to all internal variable inputs. These inputs can be formulated and determined by the decision makers.</t>
+  </si>
+  <si>
+    <t>intro_scenarios</t>
+  </si>
+  <si>
+    <t>Each external variable input can be thought of as a single aspect of external uncertainty affecting the outcome of the decision in scope. A scenario is defined by assigning a single value to all external variable inputs.</t>
+  </si>
+  <si>
+    <t>intro_fixed_inputs</t>
+  </si>
+  <si>
+    <t>The inputs which only takes one value for all scenarios.</t>
+  </si>
+  <si>
+    <t>intro_dependency_graph</t>
+  </si>
+  <si>
+    <t>intro_weighted_graph</t>
+  </si>
+  <si>
+    <t>header_theme</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>header_key_outputs</t>
+  </si>
+  <si>
+    <t>Key output</t>
+  </si>
+  <si>
+    <t>graph_title_dmo</t>
+  </si>
+  <si>
+    <t>Appreciations per option for scenario</t>
+  </si>
+  <si>
+    <t>graph_y_label_dmo</t>
+  </si>
+  <si>
+    <t>Appreciation</t>
+  </si>
+  <si>
+    <t>graph_text_dmo</t>
+  </si>
+  <si>
+    <t>The chart below shows the weighted appreciations per option, where key outputs are grouped into themes. The used theme weights are displayed in the pie chart on the right, showing the relative weights of all key outputs belonging to that theme. Use the dropdown menu to navigate through the various scenarios.</t>
+  </si>
+  <si>
+    <t>table_text_dmo</t>
+  </si>
+  <si>
+    <t>The table below shows the key output values per option, based on the selected scenario. The option with the highest weighted appreciation is highlighted.</t>
+  </si>
+  <si>
+    <t>graph_text_scenarios</t>
+  </si>
+  <si>
+    <t>The chart below shows the weighted appreciations per option, grouped into scenarios. The used scenario weights are displayed in the pie chart on the right.</t>
+  </si>
+  <si>
+    <t>graph_title_scenarios</t>
+  </si>
+  <si>
+    <t>Appreciations per scenario</t>
+  </si>
+  <si>
+    <t>graph_y_label_scenarios</t>
+  </si>
+  <si>
+    <t>Royal DSM (DSM) is a global science-based company specializing in health, nutrition, and materials. By integrating its unique expertise in Life Sciences and Materials Sciences, DSM drives economic prosperity, environmental progress, and social advancements to create sustainable value for all stakeholders. DSM operates in global markets such as food and dietary supplements, personal care, animal feed, medical devices, automotive, paints, electrical and electronics, life protection, alternative energy, and bio-based materials.
+This case explores DSM's decision-making process as the company aims to address climate change by reducing its environmental and carbon footprint through greenhouse gas emission reductions and increased energy efficiency. Their strategic challenge has been identified as determining how to source energy sustainably.</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>EN</t>
   </si>
 </sst>
 </file>
@@ -499,9 +611,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -569,6 +688,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -643,64 +769,68 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1005,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1030,6 +1160,14 @@
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1188,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E1CC75-D97A-4B40-BEB4-D0908A445A81}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1214,87 +1352,235 @@
         <v>127</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>133</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>140</v>
+      <c r="A8" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>142</v>
+      <c r="A9" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>144</v>
+      <c r="A10" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="21"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1306,31 +1592,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AD5AE-B0E9-A747-915F-4F9B572E98DB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" style="20" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changes for DSM and saving the dependency graphs
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/DSM/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mveenboer002/Dep_graph/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE116A6-F48F-6242-807A-86AD9CBFE2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78A0733-DC11-C447-9C3E-CADCEB6A7576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="-20360" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="188">
   <si>
     <t>configuration</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>Current employee recommendation rate</t>
-  </si>
-  <si>
-    <t>New Net Promotor Score</t>
   </si>
   <si>
     <t>Cost RE make</t>
@@ -608,8 +605,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -769,7 +766,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
@@ -806,7 +803,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1164,10 +1161,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1294,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -1341,7 +1338,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -1349,238 +1346,238 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>130</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>132</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>141</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>143</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>147</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>149</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>155</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>157</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>161</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>163</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B21" s="21"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" s="21"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>169</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>171</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>173</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>175</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>177</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>179</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>181</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>183</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1602,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -1613,10 +1610,10 @@
     </row>
     <row r="2" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1632,7 +1629,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1945,7 +1942,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -1956,7 +1953,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1967,7 +1964,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1978,7 +1975,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1986,10 +1983,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -1997,10 +1994,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -2008,10 +2005,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -2063,7 +2060,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>46</v>
@@ -2074,7 +2071,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>46</v>
@@ -2085,7 +2082,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>46</v>
@@ -2099,7 +2096,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -2110,7 +2107,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>0.5</v>
@@ -2121,7 +2118,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -2132,7 +2129,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
@@ -2140,10 +2137,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -2151,10 +2148,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="5">
         <v>0</v>
@@ -2162,10 +2159,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>45</v>
@@ -2228,7 +2225,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>45</v>
@@ -2239,7 +2236,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>45</v>
@@ -2294,7 +2291,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>47</v>
@@ -2305,7 +2302,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>47</v>
@@ -2316,7 +2313,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>47</v>
@@ -2375,7 +2372,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>44</v>
@@ -2387,7 +2384,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>44</v>
@@ -2399,7 +2396,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>44</v>
@@ -2448,7 +2445,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="6">
         <v>108</v>
@@ -2459,7 +2456,7 @@
         <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="6">
         <v>270</v>
@@ -2470,7 +2467,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="6">
         <v>130</v>
@@ -2481,7 +2478,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="6">
         <v>115</v>
@@ -2492,7 +2489,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="6">
         <v>51</v>
@@ -2503,7 +2500,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="6">
         <v>0.3</v>
@@ -2514,7 +2511,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="6">
         <v>0.3</v>
@@ -2989,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3039,10 +3036,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3053,10 +3050,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3084,7 +3081,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3103,7 +3100,7 @@
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
@@ -3112,12 +3109,12 @@
         <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -3126,7 +3123,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3145,7 +3142,7 @@
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>70</v>
@@ -3162,10 +3159,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>28</v>
@@ -3196,7 +3193,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3207,10 +3204,10 @@
         <v>76</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3224,7 +3221,7 @@
         <v>77</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3238,7 +3235,7 @@
         <v>49</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3266,7 +3263,7 @@
         <v>80</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3274,13 +3271,13 @@
         <v>82</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3288,13 +3285,13 @@
         <v>83</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3336,7 +3333,7 @@
         <v>82</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3378,7 +3375,7 @@
         <v>87</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3392,7 +3389,7 @@
         <v>83</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3434,12 +3431,12 @@
         <v>90</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>88</v>
@@ -3448,12 +3445,12 @@
         <v>87</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>91</v>
@@ -3462,12 +3459,12 @@
         <v>90</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -3476,7 +3473,7 @@
         <v>92</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3487,10 +3484,10 @@
         <v>68</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3509,7 +3506,7 @@
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>87</v>
@@ -3523,7 +3520,7 @@
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>84</v>
@@ -3537,7 +3534,7 @@
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>91</v>
@@ -3551,7 +3548,7 @@
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>90</v>
@@ -3565,7 +3562,7 @@
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>85</v>
@@ -3579,7 +3576,7 @@
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>93</v>
@@ -3602,7 +3599,7 @@
         <v>88</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3616,7 +3613,7 @@
         <v>91</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3655,7 +3652,7 @@
         <v>96</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>28</v>
@@ -3669,10 +3666,10 @@
         <v>94</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3680,13 +3677,13 @@
         <v>32</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>106</v>
-      </c>
       <c r="D48" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3694,13 +3691,13 @@
         <v>32</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3714,7 +3711,7 @@
         <v>89</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3728,7 +3725,7 @@
         <v>73</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3742,7 +3739,7 @@
         <v>33</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3770,7 +3767,7 @@
         <v>96</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3798,7 +3795,7 @@
         <v>59</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3817,7 +3814,7 @@
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>61</v>
@@ -3826,14 +3823,14 @@
         <v>36</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E58" s="16"/>
       <c r="F58" s="16"/>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="15">
         <v>1</v>
@@ -3842,23 +3839,23 @@
         <v>61</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E59" s="16"/>
       <c r="F59" s="16"/>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B60" s="15">
         <v>1</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
@@ -3884,7 +3881,7 @@
         <v>101</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>63</v>
@@ -3897,10 +3894,10 @@
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>69</v>
@@ -3913,10 +3910,10 @@
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>63</v>
@@ -3932,13 +3929,13 @@
         <v>37</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E65" s="16"/>
       <c r="F65" s="16"/>
@@ -3948,20 +3945,20 @@
         <v>99</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66" s="11">
         <v>0</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="16"/>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
-        <v>102</v>
+      <c r="A67" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>99</v>
@@ -3976,8 +3973,8 @@
       <c r="F67" s="16"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>102</v>
+      <c r="A68" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="B68" s="15">
         <v>0</v>
@@ -3991,19 +3988,10 @@
       <c r="E68" s="16"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>121</v>
-      </c>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
     </row>

</xml_diff>

<commit_message>
fix demo cases and warnings
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96E510B-52E3-F148-9B58-550F0A72945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114CF110-45FB-9346-9CA8-CB0A11CEA40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="181">
   <si>
     <t>configuration</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Current employee engagement score</t>
-  </si>
-  <si>
-    <t>Current Net Promotor Score</t>
   </si>
   <si>
     <t>Disengaged employee recommendation rate</t>
@@ -1134,10 +1131,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>180</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1267,7 +1264,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -1311,7 +1308,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -1319,238 +1316,238 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>136</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>140</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>142</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>152</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="20"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>174</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1572,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -1583,10 +1580,10 @@
     </row>
     <row r="2" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1602,7 +1599,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1662,12 +1659,8 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="13">
-        <v>-41400000</v>
-      </c>
-      <c r="H2" s="13">
-        <v>30000000</v>
-      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -1688,12 +1681,8 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="13">
-        <v>5734800</v>
-      </c>
-      <c r="H3" s="13">
-        <v>8389800</v>
-      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
@@ -1714,12 +1703,8 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.1</v>
-      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
@@ -1740,12 +1725,8 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>3988.3999999999942</v>
-      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -1766,12 +1747,8 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="13">
-        <v>39884</v>
-      </c>
-      <c r="H6" s="13">
-        <v>39884</v>
-      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -1792,12 +1769,8 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>1.73</v>
-      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -1818,12 +1791,8 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1.1244999999999998</v>
-      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -1844,12 +1813,8 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0.17300000000000001</v>
-      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
@@ -1870,12 +1835,8 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="13">
-        <v>0</v>
-      </c>
-      <c r="H10" s="13">
-        <v>845540.79999999877</v>
-      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1911,7 +1872,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -1922,7 +1883,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1933,7 +1894,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1944,7 +1905,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1952,10 +1913,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -1963,10 +1924,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1974,10 +1935,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -2029,7 +1990,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>40</v>
@@ -2040,7 +2001,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>40</v>
@@ -2051,7 +2012,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>40</v>
@@ -2065,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -2076,7 +2037,7 @@
         <v>37</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5">
         <v>0.5</v>
@@ -2087,7 +2048,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -2098,7 +2059,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
@@ -2106,10 +2067,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -2117,10 +2078,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="5">
         <v>0</v>
@@ -2128,10 +2089,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -2183,7 +2144,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
@@ -2194,7 +2155,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>39</v>
@@ -2205,7 +2166,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>39</v>
@@ -2260,7 +2221,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>41</v>
@@ -2271,7 +2232,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>41</v>
@@ -2282,7 +2243,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>41</v>
@@ -2341,7 +2302,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>38</v>
@@ -2353,7 +2314,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>38</v>
@@ -2365,7 +2326,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>38</v>
@@ -2414,7 +2375,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6">
         <v>108</v>
@@ -2425,7 +2386,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6">
         <v>270</v>
@@ -2436,7 +2397,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="6">
         <v>130</v>
@@ -2447,7 +2408,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="6">
         <v>115</v>
@@ -2458,7 +2419,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="6">
         <v>51</v>
@@ -2469,7 +2430,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="6">
         <v>0.3</v>
@@ -2480,7 +2441,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6">
         <v>0.3</v>
@@ -2647,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2711,7 +2672,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="8">
-        <v>0.36</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2719,7 +2680,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="8">
-        <v>0.13</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2727,7 +2688,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="8">
-        <v>212</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2735,7 +2696,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="8">
-        <v>0.1</v>
+        <v>1.7299999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2751,7 +2712,7 @@
         <v>61</v>
       </c>
       <c r="B12" s="8">
-        <v>1.7299999999999999E-2</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2759,7 +2720,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="8">
-        <v>30000</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2767,16 +2728,11 @@
         <v>63</v>
       </c>
       <c r="B14" s="8">
-        <v>0.78</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="8">
-        <v>40000000</v>
-      </c>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -2942,9 +2898,6 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2955,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
@@ -2983,41 +2936,41 @@
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>23</v>
@@ -3025,27 +2978,27 @@
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>22</v>
@@ -3053,7 +3006,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
@@ -3062,12 +3015,12 @@
         <v>48</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -3076,15 +3029,15 @@
         <v>47</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>51</v>
@@ -3095,13 +3048,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>22</v>
@@ -3112,10 +3065,10 @@
         <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>22</v>
@@ -3123,13 +3076,13 @@
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>23</v>
@@ -3137,49 +3090,49 @@
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>44</v>
@@ -3188,18 +3141,18 @@
         <v>43</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>22</v>
@@ -3207,55 +3160,55 @@
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>22</v>
@@ -3263,13 +3216,13 @@
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>22</v>
@@ -3277,27 +3230,27 @@
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>22</v>
@@ -3305,10 +3258,10 @@
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>37</v>
@@ -3319,41 +3272,41 @@
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>22</v>
@@ -3361,10 +3314,10 @@
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>35</v>
@@ -3375,80 +3328,80 @@
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>46</v>
@@ -3459,10 +3412,10 @@
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>46</v>
@@ -3473,10 +3426,10 @@
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>44</v>
@@ -3487,10 +3440,10 @@
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>45</v>
@@ -3501,10 +3454,10 @@
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>45</v>
@@ -3515,10 +3468,10 @@
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>43</v>
@@ -3529,10 +3482,10 @@
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>42</v>
@@ -3543,38 +3496,38 @@
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>54</v>
@@ -3588,7 +3541,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>54</v>
@@ -3599,13 +3552,13 @@
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>22</v>
@@ -3616,13 +3569,13 @@
         <v>26</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3630,13 +3583,13 @@
         <v>26</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="D48" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3644,13 +3597,13 @@
         <v>26</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3658,13 +3611,13 @@
         <v>27</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3675,15 +3628,15 @@
         <v>0</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" s="11">
         <v>1</v>
@@ -3692,7 +3645,7 @@
         <v>27</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3700,7 +3653,7 @@
         <v>28</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>54</v>
@@ -3717,10 +3670,10 @@
         <v>0</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3731,7 +3684,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>22</v>
@@ -3739,7 +3692,7 @@
     </row>
     <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>27</v>
@@ -3748,7 +3701,7 @@
         <v>53</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3756,10 +3709,10 @@
         <v>30</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>22</v>
@@ -3767,7 +3720,7 @@
     </row>
     <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>55</v>
@@ -3776,12 +3729,12 @@
         <v>30</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" s="15">
         <v>1</v>
@@ -3790,32 +3743,32 @@
         <v>55</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" s="15">
         <v>1</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>22</v>
@@ -3823,13 +3776,13 @@
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>22</v>
@@ -3837,13 +3790,13 @@
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>22</v>
@@ -3851,13 +3804,13 @@
     </row>
     <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>22</v>
@@ -3868,27 +3821,27 @@
         <v>31</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" s="11">
         <v>0</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3896,10 +3849,10 @@
         <v>32</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>22</v>
@@ -3913,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
fix demo cases and warnings (#106)
Co-authored-by: Thom-Ivar van Dijk <thomivar@gmail.com>
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/DSM/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96E510B-52E3-F148-9B58-550F0A72945F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114CF110-45FB-9346-9CA8-CB0A11CEA40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="181">
   <si>
     <t>configuration</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Current employee engagement score</t>
-  </si>
-  <si>
-    <t>Current Net Promotor Score</t>
   </si>
   <si>
     <t>Disengaged employee recommendation rate</t>
@@ -1134,10 +1131,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>180</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1267,7 +1264,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -1311,7 +1308,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -1319,238 +1316,238 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>136</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>140</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>142</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>152</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="20"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>174</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1572,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -1583,10 +1580,10 @@
     </row>
     <row r="2" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1602,7 +1599,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1662,12 +1659,8 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="13">
-        <v>-41400000</v>
-      </c>
-      <c r="H2" s="13">
-        <v>30000000</v>
-      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -1688,12 +1681,8 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="13">
-        <v>5734800</v>
-      </c>
-      <c r="H3" s="13">
-        <v>8389800</v>
-      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
@@ -1714,12 +1703,8 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.1</v>
-      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
@@ -1740,12 +1725,8 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>3988.3999999999942</v>
-      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -1766,12 +1747,8 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="13">
-        <v>39884</v>
-      </c>
-      <c r="H6" s="13">
-        <v>39884</v>
-      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -1792,12 +1769,8 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>1.73</v>
-      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -1818,12 +1791,8 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1.1244999999999998</v>
-      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -1844,12 +1813,8 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0.17300000000000001</v>
-      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
@@ -1870,12 +1835,8 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="13">
-        <v>0</v>
-      </c>
-      <c r="H10" s="13">
-        <v>845540.79999999877</v>
-      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1911,7 +1872,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -1922,7 +1883,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1933,7 +1894,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1944,7 +1905,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1952,10 +1913,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -1963,10 +1924,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1974,10 +1935,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -2029,7 +1990,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>40</v>
@@ -2040,7 +2001,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>40</v>
@@ -2051,7 +2012,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>40</v>
@@ -2065,7 +2026,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -2076,7 +2037,7 @@
         <v>37</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5">
         <v>0.5</v>
@@ -2087,7 +2048,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -2098,7 +2059,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
@@ -2106,10 +2067,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -2117,10 +2078,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="5">
         <v>0</v>
@@ -2128,10 +2089,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -2183,7 +2144,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
@@ -2194,7 +2155,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>39</v>
@@ -2205,7 +2166,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>39</v>
@@ -2260,7 +2221,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>41</v>
@@ -2271,7 +2232,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>41</v>
@@ -2282,7 +2243,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>41</v>
@@ -2341,7 +2302,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>38</v>
@@ -2353,7 +2314,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>38</v>
@@ -2365,7 +2326,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>38</v>
@@ -2414,7 +2375,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6">
         <v>108</v>
@@ -2425,7 +2386,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="6">
         <v>270</v>
@@ -2436,7 +2397,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="6">
         <v>130</v>
@@ -2447,7 +2408,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="6">
         <v>115</v>
@@ -2458,7 +2419,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="6">
         <v>51</v>
@@ -2469,7 +2430,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="6">
         <v>0.3</v>
@@ -2480,7 +2441,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6">
         <v>0.3</v>
@@ -2647,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2711,7 +2672,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="8">
-        <v>0.36</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2719,7 +2680,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="8">
-        <v>0.13</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2727,7 +2688,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="8">
-        <v>212</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2735,7 +2696,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="8">
-        <v>0.1</v>
+        <v>1.7299999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2751,7 +2712,7 @@
         <v>61</v>
       </c>
       <c r="B12" s="8">
-        <v>1.7299999999999999E-2</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2759,7 +2720,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="8">
-        <v>30000</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2767,16 +2728,11 @@
         <v>63</v>
       </c>
       <c r="B14" s="8">
-        <v>0.78</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="8">
-        <v>40000000</v>
-      </c>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -2942,9 +2898,6 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2955,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
@@ -2983,41 +2936,41 @@
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>23</v>
@@ -3025,27 +2978,27 @@
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>22</v>
@@ -3053,7 +3006,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
@@ -3062,12 +3015,12 @@
         <v>48</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -3076,15 +3029,15 @@
         <v>47</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>51</v>
@@ -3095,13 +3048,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>22</v>
@@ -3112,10 +3065,10 @@
         <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>22</v>
@@ -3123,13 +3076,13 @@
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>23</v>
@@ -3137,49 +3090,49 @@
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>44</v>
@@ -3188,18 +3141,18 @@
         <v>43</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>22</v>
@@ -3207,55 +3160,55 @@
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>22</v>
@@ -3263,13 +3216,13 @@
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>22</v>
@@ -3277,27 +3230,27 @@
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>22</v>
@@ -3305,10 +3258,10 @@
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>37</v>
@@ -3319,41 +3272,41 @@
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>22</v>
@@ -3361,10 +3314,10 @@
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>35</v>
@@ -3375,80 +3328,80 @@
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>46</v>
@@ -3459,10 +3412,10 @@
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>46</v>
@@ -3473,10 +3426,10 @@
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>44</v>
@@ -3487,10 +3440,10 @@
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>45</v>
@@ -3501,10 +3454,10 @@
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>45</v>
@@ -3515,10 +3468,10 @@
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>43</v>
@@ -3529,10 +3482,10 @@
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>42</v>
@@ -3543,38 +3496,38 @@
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>54</v>
@@ -3588,7 +3541,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>54</v>
@@ -3599,13 +3552,13 @@
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>22</v>
@@ -3616,13 +3569,13 @@
         <v>26</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3630,13 +3583,13 @@
         <v>26</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="D48" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3644,13 +3597,13 @@
         <v>26</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3658,13 +3611,13 @@
         <v>27</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3675,15 +3628,15 @@
         <v>0</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" s="11">
         <v>1</v>
@@ -3692,7 +3645,7 @@
         <v>27</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3700,7 +3653,7 @@
         <v>28</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>54</v>
@@ -3717,10 +3670,10 @@
         <v>0</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3731,7 +3684,7 @@
         <v>28</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>22</v>
@@ -3739,7 +3692,7 @@
     </row>
     <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>27</v>
@@ -3748,7 +3701,7 @@
         <v>53</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3756,10 +3709,10 @@
         <v>30</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>22</v>
@@ -3767,7 +3720,7 @@
     </row>
     <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>55</v>
@@ -3776,12 +3729,12 @@
         <v>30</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" s="15">
         <v>1</v>
@@ -3790,32 +3743,32 @@
         <v>55</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" s="15">
         <v>1</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>22</v>
@@ -3823,13 +3776,13 @@
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>22</v>
@@ -3837,13 +3790,13 @@
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>22</v>
@@ -3851,13 +3804,13 @@
     </row>
     <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>22</v>
@@ -3868,27 +3821,27 @@
         <v>31</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" s="11">
         <v>0</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3896,10 +3849,10 @@
         <v>32</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>22</v>
@@ -3913,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
fix in DSM case
Changed ivi % RECs from 0 to 50 in dmo Partner RE, according to the book

Co-authored-by: Thom-Ivar <138502953+thomivarvandijk@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/DSM/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lheringa001/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114CF110-45FB-9346-9CA8-CB0A11CEA40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60416EDF-AEBC-404A-9C05-6A69215E5B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -584,8 +584,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -745,7 +745,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
@@ -782,7 +782,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -808,9 +808,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{AE53C5E1-75E6-4245-B0B1-466E5639B5C7}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1848,7 +1848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2227,7 +2229,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2610,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Same fix DSM but also for JSON en CSV
</commit_message>
<xml_diff>
--- a/src/vlinder/data/DSM/xlsx/DSM.xlsx
+++ b/src/vlinder/data/DSM/xlsx/DSM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Documents/Aangepast_report/trbs/src/vlinder/data/DSM/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E45350-C8E6-8844-9C7C-641BA006889F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D0312-FE7D-4B49-B4B6-0EDCF09C036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1149,13 +1149,12 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1963,7 +1962,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C43"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2343,7 +2342,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>